<commit_message>
created board result function
</commit_message>
<xml_diff>
--- a/AI_logic_simulator.xlsx
+++ b/AI_logic_simulator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14600" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14600" windowHeight="14820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -326,8 +326,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="399">
+  <cellStyleXfs count="425">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -766,7 +792,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="399">
+  <cellStyles count="425">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -966,6 +992,19 @@
     <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1165,6 +1204,19 @@
     <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1496,8 +1548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3246,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3511,8 +3563,8 @@
         <v>0</v>
       </c>
       <c r="J3" t="str">
-        <f>"['"&amp;B3&amp;"',"&amp;C3&amp;"],"</f>
-        <v>['0001',1],</v>
+        <f>B3&amp;"a"</f>
+        <v>0001a</v>
       </c>
       <c r="K3">
         <f t="shared" ref="E3:Q3" si="1">IF(ISNUMBER(SEARCH($B3,K$1,1)),$C3,0)</f>
@@ -3708,11 +3760,11 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D17" si="2">IF(ISNUMBER(SEARCH($B4,D$1,1)),$C4,0)</f>
+        <f>IF(ISNUMBER(SEARCH($B4,D$1,1)),$C4,0)</f>
         <v>0</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:I17" si="3">IF(
+        <f t="shared" ref="E4:I17" si="2">IF(
  IF(
   ISNUMBER(SEARCH($B4,E$1,1)),$C4,0)=0,
   IF(
@@ -3725,55 +3777,55 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J17" si="4">"['"&amp;B4&amp;"',"&amp;C4&amp;"],"</f>
-        <v>['1000',1],</v>
+        <f t="shared" ref="J4:J38" si="3">B4&amp;"a"</f>
+        <v>1000a</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="E4:Q17" si="5">IF(ISNUMBER(SEARCH($B4,K$1,1)),$C4,0)</f>
+        <f t="shared" ref="E4:Q17" si="4">IF(ISNUMBER(SEARCH($B4,K$1,1)),$C4,0)</f>
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:Y17" si="6">IF(
+        <f t="shared" ref="T4:Y17" si="5">IF(
  IF(
   ISNUMBER(SEARCH($B4,T$1,1)),$C4,0)=0,
   IF(
@@ -3786,27 +3838,27 @@
         <v>0</v>
       </c>
       <c r="U4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB4">
-        <f t="shared" ref="AB4:AG17" si="7">IF(
+        <f t="shared" ref="AB4:AG17" si="6">IF(
  IF(
   ISNUMBER(SEARCH($B4,AB$1,1)),$C4,0)=0,
   IF(
@@ -3819,23 +3871,23 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3848,107 +3900,107 @@
         <v>2</v>
       </c>
       <c r="D5">
+        <f t="shared" ref="D4:D17" si="7">IF(ISNUMBER(SEARCH($B5,D$1,1)),$C5,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E5">
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="4"/>
-        <v>['0010',2],</v>
+        <v>0010a</v>
       </c>
       <c r="K5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3961,107 +4013,107 @@
         <v>2</v>
       </c>
       <c r="D6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E6">
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="4"/>
-        <v>['0100',2],</v>
+        <v>0100a</v>
       </c>
       <c r="K6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4076,107 +4128,107 @@
         <v>5</v>
       </c>
       <c r="D7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J7" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="4"/>
-        <v>['0101',5],</v>
+        <v>0101a</v>
       </c>
       <c r="K7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4189,107 +4241,107 @@
         <v>5</v>
       </c>
       <c r="D8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E8">
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="4"/>
-        <v>['1010',5],</v>
+        <v>1010a</v>
       </c>
       <c r="K8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4302,107 +4354,107 @@
         <v>5</v>
       </c>
       <c r="D9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="4"/>
-        <v>['1001',5],</v>
+        <v>1001a</v>
       </c>
       <c r="K9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4415,107 +4467,107 @@
         <v>6</v>
       </c>
       <c r="D10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E10">
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="4"/>
-        <v>['0011',6],</v>
+        <v>0011a</v>
       </c>
       <c r="K10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="N10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4528,107 +4580,107 @@
         <v>6</v>
       </c>
       <c r="D11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E11">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="4"/>
-        <v>['1100',6],</v>
+        <v>1100a</v>
       </c>
       <c r="K11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4641,107 +4693,107 @@
         <v>13</v>
       </c>
       <c r="D12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12">
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="4"/>
-        <v>['0110',13],</v>
+        <v>0110a</v>
       </c>
       <c r="K12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>6.5</v>
       </c>
       <c r="W12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4756,107 +4808,107 @@
         <v>15</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="4"/>
-        <v>['0111',15],</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AC13">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AD13">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="3"/>
+        <v>0111a</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
       <c r="AE13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4869,107 +4921,107 @@
         <v>15</v>
       </c>
       <c r="D14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E14">
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="4"/>
-        <v>['1011',15],</v>
+        <v>1011a</v>
       </c>
       <c r="K14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -4982,107 +5034,107 @@
         <v>15</v>
       </c>
       <c r="D15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E15">
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J15" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="4"/>
-        <v>['1101',15],</v>
+        <v>1101a</v>
       </c>
       <c r="K15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -5095,107 +5147,107 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <f t="shared" si="2"/>
-        <v>15</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="4"/>
-        <v>['1110',15],</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Y16">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AB16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AC16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AD16">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="3"/>
+        <v>1110a</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
       <c r="AE16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -5210,103 +5262,103 @@
         <v>500</v>
       </c>
       <c r="D17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E17">
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="4"/>
-        <v>['1111',500],</v>
+        <v>1111a</v>
       </c>
       <c r="K17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG17">
@@ -5323,6 +5375,12 @@
         <v>0</v>
       </c>
     </row>
+    <row r="18" spans="1:33">
+      <c r="J18" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+    </row>
     <row r="19" spans="1:33">
       <c r="A19" t="s">
         <v>20</v>
@@ -5332,6 +5390,10 @@
       </c>
       <c r="C19" t="s">
         <v>24</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="3"/>
+        <v>Permutationsa</v>
       </c>
     </row>
     <row r="20" spans="1:33">
@@ -5378,39 +5440,39 @@
         <v>0</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ref="J20:J27" si="9">"['"&amp;B20&amp;"',"&amp;C20&amp;"],"</f>
-        <v>['00010',1],</v>
+        <f t="shared" si="3"/>
+        <v>00010a</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="E20:Q20" si="10">IF(ISNUMBER(SEARCH($B20,K$1,1)),$C20,0)</f>
+        <f t="shared" ref="E20:Q20" si="9">IF(ISNUMBER(SEARCH($B20,K$1,1)),$C20,0)</f>
         <v>0</v>
       </c>
       <c r="L20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T20">
-        <f t="shared" ref="T20:Y27" si="11">IF(
+        <f t="shared" ref="T20:Y27" si="10">IF(
  IF(
   ISNUMBER(SEARCH($B20,T$1,1)),$C20,0)=0,
   IF(
@@ -5423,27 +5485,27 @@
         <v>0</v>
       </c>
       <c r="U20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="V20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="W20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="X20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AB20">
-        <f t="shared" ref="AB20:AG27" si="12">IF(
+        <f t="shared" ref="AB20:AG27" si="11">IF(
  IF(
   ISNUMBER(SEARCH($B20,AB$1,1)),$C20,0)=0,
   IF(
@@ -5456,23 +5518,23 @@
         <v>0</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AF20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -5485,7 +5547,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <f t="shared" ref="D21:Q27" si="13">IF(ISNUMBER(SEARCH($B21,D$1,1)),$C21,0)</f>
+        <f t="shared" ref="D21:Q27" si="12">IF(ISNUMBER(SEARCH($B21,D$1,1)),$C21,0)</f>
         <v>0</v>
       </c>
       <c r="E21">
@@ -5509,83 +5571,83 @@
         <v>0</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="9"/>
-        <v>['01000',1],</v>
+        <f t="shared" si="3"/>
+        <v>01000a</v>
       </c>
       <c r="K21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U21">
+      <c r="AC21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V21">
+      <c r="AD21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W21">
+      <c r="AE21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X21">
+      <c r="AF21">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y21">
+      <c r="AG21">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD21">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF21">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG21">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -5598,7 +5660,7 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E22">
@@ -5622,83 +5684,83 @@
         <v>0</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="9"/>
-        <v>['00100',2],</v>
+        <f t="shared" si="3"/>
+        <v>00100a</v>
       </c>
       <c r="K22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U22">
+      <c r="AC22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V22">
+      <c r="AD22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W22">
+      <c r="AE22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X22">
+      <c r="AF22">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y22">
+      <c r="AG22">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB22">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC22">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD22">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE22">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF22">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG22">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -5713,7 +5775,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E23">
@@ -5737,83 +5799,83 @@
         <v>0</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="9"/>
-        <v>['01010',2],</v>
+        <f t="shared" si="3"/>
+        <v>01010a</v>
       </c>
       <c r="K23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U23">
+      <c r="AC23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V23">
+      <c r="AD23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W23">
+      <c r="AE23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X23">
+      <c r="AF23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y23">
+      <c r="AG23">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB23">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC23">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF23">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -5826,7 +5888,7 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E24">
@@ -5850,83 +5912,83 @@
         <v>0</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="9"/>
-        <v>['00110',3],</v>
+        <f t="shared" si="3"/>
+        <v>00110a</v>
       </c>
       <c r="K24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U24">
+      <c r="AC24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V24">
+      <c r="AD24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W24">
+      <c r="AE24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X24">
+      <c r="AF24">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y24">
+      <c r="AG24">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF24">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG24">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -5939,7 +6001,7 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="E25">
@@ -5963,83 +6025,83 @@
         <v>0</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="9"/>
-        <v>['01100',3],</v>
+        <f t="shared" si="3"/>
+        <v>01100a</v>
       </c>
       <c r="K25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U25">
+      <c r="AC25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V25">
+      <c r="AD25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W25">
+      <c r="AE25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X25">
+      <c r="AF25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y25">
+      <c r="AG25">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB25">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC25">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD25">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AE25">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF25">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG25">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6054,7 +6116,7 @@
         <v>400</v>
       </c>
       <c r="D26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="E26">
@@ -6078,83 +6140,83 @@
         <v>0</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" si="9"/>
-        <v>['01110',400],</v>
+        <f t="shared" si="3"/>
+        <v>01110a</v>
       </c>
       <c r="K26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U26">
+      <c r="AC26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V26">
+      <c r="AD26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="W26">
+        <v>400</v>
+      </c>
+      <c r="AE26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X26">
+      <c r="AF26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y26">
+      <c r="AG26">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AB26">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC26">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <f t="shared" si="12"/>
-        <v>400</v>
-      </c>
-      <c r="AE26">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF26">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG26">
-        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -6167,7 +6229,7 @@
         <v>400</v>
       </c>
       <c r="D27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="E27">
@@ -6191,84 +6253,90 @@
         <v>0</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" si="9"/>
-        <v>['01110',400],</v>
+        <f t="shared" si="3"/>
+        <v>01110a</v>
       </c>
       <c r="K27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="L27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="N27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="T27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AB27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="U27">
+      <c r="AC27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V27">
+      <c r="AD27">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="W27">
+        <v>400</v>
+      </c>
+      <c r="AE27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="X27">
+      <c r="AF27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="Y27">
+      <c r="AG27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AB27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <f t="shared" si="12"/>
-        <v>400</v>
-      </c>
-      <c r="AE27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AF27">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AG27">
-        <f t="shared" si="12"/>
-        <v>0</v>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="J28" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
       </c>
     </row>
     <row r="29" spans="1:33">
@@ -6281,6 +6349,10 @@
       <c r="C29" t="s">
         <v>24</v>
       </c>
+      <c r="J29" t="str">
+        <f t="shared" si="3"/>
+        <v>Permutationsa</v>
+      </c>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="14">
@@ -6297,7 +6369,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30:I38" si="14">IF(
+        <f t="shared" ref="E30:I38" si="13">IF(
  IF(
   ISNUMBER(SEARCH($B30,E$1,1)),$C30,0)=0,
   IF(
@@ -6310,55 +6382,55 @@
         <v>0</v>
       </c>
       <c r="F30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" si="3"/>
+        <v>000010a</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ref="E30:Q30" si="14">IF(ISNUMBER(SEARCH($B30,K$1,1)),$C30,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G30">
+      <c r="M30">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H30">
+      <c r="N30">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I30">
+      <c r="O30">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="J30" t="str">
-        <f t="shared" ref="J30:J38" si="15">"['"&amp;B30&amp;"',"&amp;C30&amp;"],"</f>
-        <v>['000010',1],</v>
-      </c>
-      <c r="K30">
-        <f t="shared" ref="E30:Q30" si="16">IF(ISNUMBER(SEARCH($B30,K$1,1)),$C30,0)</f>
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
       <c r="P30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="T30">
-        <f t="shared" ref="T30:Y38" si="17">IF(
+        <f t="shared" ref="T30:Y38" si="15">IF(
  IF(
   ISNUMBER(SEARCH($B30,T$1,1)),$C30,0)=0,
   IF(
@@ -6371,27 +6443,27 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB30">
-        <f t="shared" ref="AB30:AG38" si="18">IF(
+        <f t="shared" ref="AB30:AG38" si="16">IF(
  IF(
   ISNUMBER(SEARCH($B30,AB$1,1)),$C30,0)=0,
   IF(
@@ -6404,23 +6476,23 @@
         <v>0</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6433,107 +6505,107 @@
         <v>1</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:Q38" si="19">IF(ISNUMBER(SEARCH($B31,D$1,1)),$C31,0)</f>
+        <f t="shared" ref="D31:Q38" si="17">IF(ISNUMBER(SEARCH($B31,D$1,1)),$C31,0)</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J31" t="str">
+        <f t="shared" si="3"/>
+        <v>010000a</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T31">
         <f t="shared" si="15"/>
-        <v>['010000',1],</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6546,107 +6618,107 @@
         <v>2</v>
       </c>
       <c r="D32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J32" t="str">
+        <f t="shared" si="3"/>
+        <v>001000a</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T32">
         <f t="shared" si="15"/>
-        <v>['001000',2],</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6659,107 +6731,107 @@
         <v>2</v>
       </c>
       <c r="D33">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J33" t="str">
+        <f t="shared" si="3"/>
+        <v>000100a</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T33">
         <f t="shared" si="15"/>
-        <v>['000100',2],</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6774,107 +6846,107 @@
         <v>3</v>
       </c>
       <c r="D34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J34" t="str">
+        <f t="shared" si="3"/>
+        <v>000110a</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T34">
         <f t="shared" si="15"/>
-        <v>['000110',3],</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T34">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -6887,107 +6959,107 @@
         <v>4</v>
       </c>
       <c r="D35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J35" t="str">
+        <f t="shared" si="3"/>
+        <v>011000a</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T35">
         <f t="shared" si="15"/>
-        <v>['011000',4],</v>
-      </c>
-      <c r="K35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T35">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -7000,107 +7072,107 @@
         <v>4</v>
       </c>
       <c r="D36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J36" t="str">
+        <f t="shared" si="3"/>
+        <v>001100a</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T36">
         <f t="shared" si="15"/>
-        <v>['001100',4],</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T36">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -7115,107 +7187,107 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J37" t="str">
+        <f t="shared" si="3"/>
+        <v>010110a</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T37">
         <f t="shared" si="15"/>
-        <v>['010110',1],</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q37">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>
@@ -7228,107 +7300,107 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="J38" t="str">
+        <f t="shared" si="3"/>
+        <v>011010a</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="T38">
         <f t="shared" si="15"/>
-        <v>['011010',1],</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="O38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="Q38">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="U38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AD38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AF38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AG38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>